<commit_message>
Fix testfile and update requirements
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guthrieec/Nextcloud/Albatross/EzPyZ/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF99396-0284-D548-8A47-C2FF4FA43F6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3833EA25-95D2-DE4F-B7A4-1E21492F2B9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41320" yWindow="2080" windowWidth="28040" windowHeight="17440" xr2:uid="{B80C3682-442A-CF41-A4D5-3BF5753A7368}"/>
   </bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>